<commit_message>
Update: Chi phi mua do
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\KLTN\Documents\ChiPhi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\KLTN\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BAB02CA1-AD1A-4B1C-A5A4-3658EF6093FC}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074A4D1B-5A23-4546-A1FC-0116A3F7E531}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="7464" xr2:uid="{220A58DF-6CD1-4074-9AE3-8CCB10910C50}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
   <si>
     <t>Ngày</t>
   </si>
@@ -37,6 +37,15 @@
   </si>
   <si>
     <t>MPU6050 x3</t>
+  </si>
+  <si>
+    <t>HM-10</t>
+  </si>
+  <si>
+    <t>Pin LIPO 500mAh</t>
+  </si>
+  <si>
+    <t>Mạch sạc pin LIPO</t>
   </si>
 </sst>
 </file>
@@ -101,7 +110,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -113,6 +122,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -429,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E42E516-3BB6-43DF-9B79-28ADEF8E1CD7}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -462,6 +474,50 @@
         <v>147000</v>
       </c>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3" s="5">
+        <v>43178</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="1">
+        <v>115000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4" s="5">
+        <v>43178</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="1">
+        <v>55000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5" s="5">
+        <v>43179</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="1">
+        <v>15000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" s="5">
+        <v>43181</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="1">
+        <v>115000</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Update: Them chi phi mua the sdcard cho raspberry
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\KLTN\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074A4D1B-5A23-4546-A1FC-0116A3F7E531}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091B2DD4-738E-47A0-A01E-3B992DC3750C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="7464" xr2:uid="{220A58DF-6CD1-4074-9AE3-8CCB10910C50}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>Ngày</t>
   </si>
@@ -46,6 +46,15 @@
   </si>
   <si>
     <t>Mạch sạc pin LIPO</t>
+  </si>
+  <si>
+    <t>MicroSD 16GB</t>
+  </si>
+  <si>
+    <t>Chú thích</t>
+  </si>
+  <si>
+    <t>https://memoryzone.com.vn/the-nho-microsdhc-sandisk-ultra-16gb-80mbs-533x-2017/</t>
   </si>
 </sst>
 </file>
@@ -110,7 +119,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -124,9 +133,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -441,18 +452,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E42E516-3BB6-43DF-9B79-28ADEF8E1CD7}">
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="3" width="15.77734375" style="1" customWidth="1"/>
+    <col min="4" max="4" width="83.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -462,60 +474,82 @@
       <c r="C1" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43165</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="3">
+      <c r="C2" s="6">
         <v>147000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" s="5">
+      <c r="D2" s="5"/>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3" s="2">
         <v>43178</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="1">
+      <c r="C3" s="6">
         <v>115000</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" s="5">
+      <c r="D3" s="5"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4" s="2">
         <v>43178</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="1">
+      <c r="C4" s="6">
         <v>55000</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" s="5">
+      <c r="D4" s="5"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>43179</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="1">
+      <c r="C5" s="6">
         <v>15000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" s="5">
+      <c r="D5" s="5"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>43181</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="1">
+      <c r="C6" s="6">
         <v>115000</v>
+      </c>
+      <c r="D6" s="5"/>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
+        <v>43187</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="6">
+        <v>170000</v>
+      </c>
+      <c r="D7" s="7" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Them chi phi mua GPS Quectel L70
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\KLTN\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{091B2DD4-738E-47A0-A01E-3B992DC3750C}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3D2D1D-5237-47BD-B54D-1621328B6890}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="7464" xr2:uid="{220A58DF-6CD1-4074-9AE3-8CCB10910C50}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
   <si>
     <t>Ngày</t>
   </si>
@@ -55,6 +55,24 @@
   </si>
   <si>
     <t>https://memoryzone.com.vn/the-nho-microsdhc-sandisk-ultra-16gb-80mbs-533x-2017/</t>
+  </si>
+  <si>
+    <t>Quectel L70 x3</t>
+  </si>
+  <si>
+    <t>http://thegioiic.com/products/gps-l70</t>
+  </si>
+  <si>
+    <t>http://hshop.vn/products/mach-thu-phat-bluetooth-4-0uart-hm10uart-chua-ra-chon</t>
+  </si>
+  <si>
+    <t>http://hshop.vn/products/cam-bien-6-dof-bac-tu-do-gy-521-mpu6050</t>
+  </si>
+  <si>
+    <t>http://hshop.vn/products/pin-lipo-3-7v1cell-600mah-20c</t>
+  </si>
+  <si>
+    <t>http://hshop.vn/products/mach-sac-pin-lithium1a-v2</t>
   </si>
 </sst>
 </file>
@@ -119,7 +137,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -138,6 +156,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -452,15 +476,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E42E516-3BB6-43DF-9B79-28ADEF8E1CD7}">
-  <dimension ref="A1:D7"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="3" width="15.77734375" style="1" customWidth="1"/>
+    <col min="1" max="2" width="15.77734375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.77734375" style="9" customWidth="1"/>
     <col min="4" max="4" width="83.88671875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -471,7 +496,7 @@
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="8" t="s">
         <v>2</v>
       </c>
       <c r="D1" s="4" t="s">
@@ -486,9 +511,12 @@
         <v>3</v>
       </c>
       <c r="C2" s="6">
+        <f>49000*3</f>
         <v>147000</v>
       </c>
-      <c r="D2" s="5"/>
+      <c r="D2" s="5" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
@@ -500,7 +528,9 @@
       <c r="C3" s="6">
         <v>115000</v>
       </c>
-      <c r="D3" s="5"/>
+      <c r="D3" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
@@ -512,7 +542,9 @@
       <c r="C4" s="6">
         <v>55000</v>
       </c>
-      <c r="D4" s="5"/>
+      <c r="D4" s="5" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
@@ -524,7 +556,9 @@
       <c r="C5" s="6">
         <v>15000</v>
       </c>
-      <c r="D5" s="5"/>
+      <c r="D5" s="5" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
@@ -536,7 +570,9 @@
       <c r="C6" s="6">
         <v>115000</v>
       </c>
-      <c r="D6" s="5"/>
+      <c r="D6" s="5" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
@@ -550,6 +586,21 @@
       </c>
       <c r="D7" s="7" t="s">
         <v>9</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
+        <v>43188</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="6">
+        <f>168000*3</f>
+        <v>504000</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: Them tien mua USB UART FT232
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyProject\KLTN\Documents\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thaonguyen\Desktop\KLTN\-KLTN-TrackingDeviceForDementiaPatients\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0C3D2D1D-5237-47BD-B54D-1621328B6890}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B199A2-B444-4E52-879C-8291F9773130}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="7464" xr2:uid="{220A58DF-6CD1-4074-9AE3-8CCB10910C50}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="7470" xr2:uid="{220A58DF-6CD1-4074-9AE3-8CCB10910C50}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Ngày</t>
   </si>
@@ -73,6 +73,12 @@
   </si>
   <si>
     <t>http://hshop.vn/products/mach-sac-pin-lithium1a-v2</t>
+  </si>
+  <si>
+    <t>USB Serial FT232</t>
+  </si>
+  <si>
+    <t>https://icdayroi.com/mach-chuyen-usb-uart-ttl-ft232rl</t>
   </si>
 </sst>
 </file>
@@ -476,20 +482,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E42E516-3BB6-43DF-9B79-28ADEF8E1CD7}">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.77734375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.77734375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="83.88671875" customWidth="1"/>
+    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.7109375" style="9" customWidth="1"/>
+    <col min="4" max="4" width="83.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -503,7 +509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>43165</v>
       </c>
@@ -518,7 +524,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>43178</v>
       </c>
@@ -532,7 +538,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>43178</v>
       </c>
@@ -546,7 +552,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>43179</v>
       </c>
@@ -560,7 +566,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>43181</v>
       </c>
@@ -574,7 +580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>43187</v>
       </c>
@@ -588,7 +594,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>43188</v>
       </c>
@@ -601,6 +607,20 @@
       </c>
       <c r="D8" s="5" t="s">
         <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>43195</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" s="6">
+        <v>60000</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update: chi phi mua do lam mach LoRa
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -1,21 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thaonguyen\Desktop\KLTN\-KLTN-TrackingDeviceForDementiaPatients\Documents\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuy Chon\Desktop\ThaoNguyen\KLTN\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15B199A2-B444-4E52-879C-8291F9773130}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="7470" xr2:uid="{220A58DF-6CD1-4074-9AE3-8CCB10910C50}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="7470"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
   <si>
     <t>Ngày</t>
   </si>
@@ -79,13 +78,31 @@
   </si>
   <si>
     <t>https://icdayroi.com/mach-chuyen-usb-uart-ttl-ft232rl</t>
+  </si>
+  <si>
+    <t>Điện trở 2K 0805 + Tụ 10uF 0805</t>
+  </si>
+  <si>
+    <t>http://thegioiic.com/</t>
+  </si>
+  <si>
+    <t>Bảo tín</t>
+  </si>
+  <si>
+    <t>Diode 1N4007 + Nút + Lưỡi cưa mạch + Bút lông</t>
+  </si>
+  <si>
+    <t>GPS Ublox Neo7</t>
+  </si>
+  <si>
+    <t>http://hshop.vn/products/mach-gps-ublox-neo-7</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -97,6 +114,14 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -140,10 +165,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -168,8 +194,11 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -481,16 +510,17 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E42E516-3BB6-43DF-9B79-28ADEF8E1CD7}">
-  <dimension ref="A1:D9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="15.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="9" customWidth="1"/>
     <col min="4" max="4" width="83.85546875" customWidth="1"/>
   </cols>
@@ -623,8 +653,51 @@
         <v>17</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2"/>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="6">
+        <v>380000</v>
+      </c>
+      <c r="D10" s="11" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>43237</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="6">
+        <v>65000</v>
+      </c>
+      <c r="D11" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>43238</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="6">
+        <v>14800</v>
+      </c>
+      <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D10" r:id="rId1"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update: Them chi phi mua do lam mach LoRa
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="18431"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuy Chon\Desktop\ThaoNguyen\KLTN\Documents\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\TechMaster\Desktop\ThaoNguyen\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,7 +14,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="171027"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="25">
   <si>
     <t>Ngày</t>
   </si>
@@ -96,12 +96,15 @@
   </si>
   <si>
     <t>http://hshop.vn/products/mach-gps-ublox-neo-7</t>
+  </si>
+  <si>
+    <t>Tụ 10uF + Diode 1N4007 + Nhíp kẹp linh kiện + Atmeage 328p</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -198,8 +201,8 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
+    <cellStyle name="Siêu kết nối" xfId="1" builtinId="8"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -511,16 +514,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="34.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="15.7109375" style="9" customWidth="1"/>
     <col min="4" max="4" width="83.85546875" customWidth="1"/>
   </cols>
@@ -690,6 +693,20 @@
         <v>14800</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>43239</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="6">
+        <v>223500</v>
+      </c>
+      <c r="D13" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Update: Them tai lieu ve module LoRa SX1280 2.4GHz
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19226"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuy Chon\Desktop\ThaoNguyen\KLTN\Documents\Cost\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ThaoNguyen\Workspace\KLTN\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D5C729-6322-4761-BA2A-D46BCE44CF77}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12930" windowHeight="7470"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="7476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="179017"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Ngày</t>
   </si>
@@ -102,13 +103,16 @@
   </si>
   <si>
     <t>Tụ 100nF + Atmega328</t>
+  </si>
+  <si>
+    <t>In mạch burn bootloader Atmega328 + 10 led đỏ 5mm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -132,6 +136,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -147,7 +166,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -170,12 +189,34 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -202,6 +243,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -516,22 +573,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.7109375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="66.7109375" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.7109375" style="9" customWidth="1"/>
-    <col min="4" max="4" width="83.85546875" customWidth="1"/>
+    <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="66.6640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="9" customWidth="1"/>
+    <col min="4" max="4" width="83.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
@@ -545,7 +602,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>43165</v>
       </c>
@@ -560,7 +617,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>43178</v>
       </c>
@@ -574,7 +631,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>43178</v>
       </c>
@@ -588,7 +645,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>43179</v>
       </c>
@@ -602,7 +659,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>43181</v>
       </c>
@@ -616,7 +673,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>43187</v>
       </c>
@@ -630,7 +687,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>43188</v>
       </c>
@@ -645,7 +702,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>43195</v>
       </c>
@@ -659,7 +716,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" s="2"/>
       <c r="B10" s="3" t="s">
         <v>22</v>
@@ -671,7 +728,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>43237</v>
       </c>
@@ -685,7 +742,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>43238</v>
       </c>
@@ -699,7 +756,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>43239</v>
       </c>
@@ -713,7 +770,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>43242</v>
       </c>
@@ -727,9 +784,32 @@
         <v>19</v>
       </c>
     </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A15" s="15">
+        <v>43242</v>
+      </c>
+      <c r="B15" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="13">
+        <v>15000</v>
+      </c>
+      <c r="D15" s="10" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="14"/>
+      <c r="D16" s="12"/>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+      <c r="B21"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Thêm chi phí mua Arduino Nano và linh kiện làm mạch test module Sx1280
</commit_message>
<xml_diff>
--- a/Documents/Cost/ChiPhi.xlsx
+++ b/Documents/Cost/ChiPhi.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ThaoNguyen\Workspace\KLTN\Documents\Cost\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B6D5C729-6322-4761-BA2A-D46BCE44CF77}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{718B9A81-CE82-4FF1-9D59-6313399517FA}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="7476" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="30">
   <si>
     <t>Ngày</t>
   </si>
@@ -106,13 +106,22 @@
   </si>
   <si>
     <t>In mạch burn bootloader Atmega328 + 10 led đỏ 5mm</t>
+  </si>
+  <si>
+    <t>https://icdayroi.com/arduino-nano-v3-0-atmega328p</t>
+  </si>
+  <si>
+    <t>Arduino nano V3.0 ATmega328P x2</t>
+  </si>
+  <si>
+    <t>In mạch, board đồng, nước rửa mạch, rào cái vuông x4</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -129,24 +138,7 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -166,7 +158,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -189,79 +181,40 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="3" fontId="3" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -577,239 +530,261 @@
   <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="15.6640625" style="1" customWidth="1"/>
     <col min="2" max="2" width="66.6640625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" style="9" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" style="4" customWidth="1"/>
     <col min="4" max="4" width="83.88671875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="18" x14ac:dyDescent="0.3">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="2" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A2" s="2">
+      <c r="A2" s="5">
         <v>43165</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="6">
+      <c r="C2" s="7">
         <f>49000*3</f>
         <v>147000</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A3" s="2">
+      <c r="A3" s="5">
         <v>43178</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="6">
+      <c r="C3" s="7">
         <v>115000</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A4" s="2">
+      <c r="A4" s="5">
         <v>43178</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="6">
+      <c r="C4" s="7">
         <v>55000</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="8" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A5" s="2">
+      <c r="A5" s="5">
         <v>43179</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="6">
+      <c r="C5" s="7">
         <v>15000</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="8" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A6" s="2">
+      <c r="A6" s="5">
         <v>43181</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="6">
+      <c r="C6" s="7">
         <v>115000</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="8" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A7" s="2">
+      <c r="A7" s="5">
         <v>43187</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="6">
+      <c r="C7" s="7">
         <v>170000</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D7" s="8" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A8" s="2">
+      <c r="A8" s="5">
         <v>43188</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C8" s="6">
+      <c r="C8" s="7">
         <f>168000*3</f>
         <v>504000</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="8" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A9" s="2">
+      <c r="A9" s="5">
         <v>43195</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="6">
+      <c r="C9" s="7">
         <v>60000</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="8" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="3" t="s">
+      <c r="A10" s="5"/>
+      <c r="B10" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C10" s="6">
+      <c r="C10" s="7">
         <v>380000</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A11" s="2">
+      <c r="A11" s="5">
         <v>43237</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="6">
+      <c r="C11" s="7">
         <v>65000</v>
       </c>
-      <c r="D11" s="10" t="s">
+      <c r="D11" s="9" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A12" s="2">
+      <c r="A12" s="5">
         <v>43238</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C12" s="6">
+      <c r="C12" s="7">
         <v>14800</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A13" s="2">
+      <c r="A13" s="5">
         <v>43239</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C13" s="6">
+      <c r="C13" s="7">
         <v>223500</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A14" s="2">
+      <c r="A14" s="5">
         <v>43242</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="6">
+      <c r="C14" s="7">
         <v>65500</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="8" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.3">
-      <c r="A15" s="15">
+      <c r="A15" s="5">
         <v>43242</v>
       </c>
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="7">
         <v>15000</v>
       </c>
-      <c r="D15" s="10" t="s">
+      <c r="D15" s="9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="17"/>
-      <c r="B16" s="17"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="12"/>
-    </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="5">
+        <v>43246</v>
+      </c>
+      <c r="B16" s="10" t="s">
+        <v>28</v>
+      </c>
+      <c r="C16" s="7">
+        <v>120000</v>
+      </c>
+      <c r="D16" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A17" s="5">
+        <v>43246</v>
+      </c>
+      <c r="B17" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="C17" s="7">
+        <v>50000</v>
+      </c>
+      <c r="D17" s="9" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="B21"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId1" xr:uid="{B31838E3-3F2F-4110-B448-6C648124988F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>